<commit_message>
edit field defined movies
</commit_message>
<xml_diff>
--- a/document/Design/Field Definition/Field_Defined_Movie.xlsx
+++ b/document/Design/Field Definition/Field_Defined_Movie.xlsx
@@ -310,13 +310,6 @@
     <t>SCREEN CODE</t>
   </si>
   <si>
-    <t>กรณีสามารถค้นหาได้
-- Word Search
-- Limit 20 Movies
-กรณีไม่สามารถค้นหาได้
-- บัญชีผู้ใช้ถูกระงับการใช้งาน</t>
-  </si>
-  <si>
     <t>Modal</t>
   </si>
   <si>
@@ -398,6 +391,13 @@
   </si>
   <si>
     <t>lang_th</t>
+  </si>
+  <si>
+    <t>กรณีสามารถค้นหาได้
+- Word Search
+- Limit 10 Movies
+กรณีไม่สามารถค้นหาได้
+- บัญชีผู้ใช้ถูกระงับการใช้งาน</t>
   </si>
 </sst>
 </file>
@@ -689,29 +689,29 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37:N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1025,10 +1025,10 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -1036,10 +1036,10 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
@@ -1047,10 +1047,10 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
@@ -1058,10 +1058,10 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
@@ -1069,10 +1069,10 @@
       <c r="A5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
@@ -1409,7 +1409,7 @@
         <v>73</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="13"/>
     </row>
@@ -1446,7 +1446,7 @@
         <v>73</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q17" s="13"/>
     </row>
@@ -1455,13 +1455,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="11"/>
@@ -1483,7 +1483,7 @@
         <v>73</v>
       </c>
       <c r="P18" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q18" s="13"/>
     </row>
@@ -1492,13 +1492,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="11"/>
@@ -1520,7 +1520,7 @@
         <v>73</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q19" s="13"/>
     </row>
@@ -1529,7 +1529,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
@@ -1562,7 +1562,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12" t="s">
@@ -1801,10 +1801,10 @@
       <c r="D30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="25"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="8" t="s">
         <v>25</v>
       </c>
@@ -1942,12 +1942,12 @@
         <v>48</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
+        <v>116</v>
+      </c>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
       <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" ht="66" customHeight="1">
@@ -1964,7 +1964,7 @@
         <v>55</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="13" t="s">
@@ -1974,12 +1974,12 @@
         <v>48</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
+        <v>94</v>
+      </c>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
       <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" ht="66" customHeight="1">
@@ -1996,7 +1996,7 @@
         <v>58</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="13" t="s">
@@ -2006,12 +2006,12 @@
         <v>48</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
       <c r="N38" s="17"/>
     </row>
     <row r="39" spans="1:14" ht="112.5" customHeight="1">
@@ -2028,22 +2028,22 @@
         <v>77</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>48</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
+        <v>106</v>
+      </c>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
       <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" ht="66" customHeight="1">
@@ -2060,22 +2060,22 @@
         <v>76</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>48</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
+        <v>107</v>
+      </c>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
       <c r="N40" s="17"/>
     </row>
     <row r="41" spans="1:14" ht="66" customHeight="1">
@@ -2092,22 +2092,22 @@
         <v>80</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>48</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
+        <v>108</v>
+      </c>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
       <c r="N41" s="17"/>
     </row>
     <row r="42" spans="1:14">
@@ -2115,33 +2115,50 @@
         <v>10.1</v>
       </c>
       <c r="B42" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="D42" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="E42" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>113</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="13" t="s">
         <v>27</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I42" s="16"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
       <c r="N42" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="I40:N40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="I41:N41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="I42:N42"/>
+    <mergeCell ref="I36:N36"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="I37:N37"/>
+    <mergeCell ref="I38:N38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -2149,23 +2166,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="I36:N36"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="I37:N37"/>
-    <mergeCell ref="I38:N38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="I39:N39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="I40:N40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="I41:N41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="I42:N42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5:C5" r:id="rId1" display="movies_list"/>

</xml_diff>